<commit_message>
updated excel upload template for vending requests
</commit_message>
<xml_diff>
--- a/public/vending-request-excel-template.xlsx
+++ b/public/vending-request-excel-template.xlsx
@@ -1,53 +1,73 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lhobbs\Documents\dev\cti_blog_next\cti_blog\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\balder\user folders\lhobbs\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88B0ACC0-5C07-46A4-90B7-1861C106FAAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA36E96-4D7E-41ED-B471-6E1842DA176A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34065" yWindow="2475" windowWidth="19710" windowHeight="12870" xr2:uid="{C3930CCD-CC11-4EF9-B7C0-BA42E04FA4AD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="vending_request_upload_template" sheetId="1" r:id="rId1"/>
+    <sheet name="price_types" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Min</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>Requested By</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>description_1</t>
+  </si>
+  <si>
+    <t>description_2</t>
+  </si>
+  <si>
+    <t>sales_rep</t>
+  </si>
+  <si>
+    <t>supply_net_number</t>
+  </si>
+  <si>
+    <t>mfg</t>
+  </si>
+  <si>
+    <t>mfg_number</t>
+  </si>
+  <si>
+    <t>issue_qty</t>
+  </si>
+  <si>
+    <t>margin</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>price_type</t>
+  </si>
+  <si>
+    <t>profit</t>
+  </si>
+  <si>
+    <t>customer</t>
   </si>
 </sst>
 </file>
@@ -119,7 +139,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -131,7 +151,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -178,23 +198,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -230,23 +233,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -398,33 +384,101 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C2AEBC6-2F6D-4F3C-A49B-E06C7D38AC4A}">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="K1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C0C977AC-A513-4D2B-8C32-26BA4CFD6B3B}">
+          <x14:formula1>
+            <xm:f>price_types!$A$1:$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C0EB62-6305-475D-8AAE-3352D7D9B6B5}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vending upload request data validation
</commit_message>
<xml_diff>
--- a/public/vending-request-excel-template.xlsx
+++ b/public/vending-request-excel-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14234\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14234\OneDrive\Desktop\Web Dev\Projects\cti_blog\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{91C36D27-B049-4A3E-8F90-52CCC8B5F8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BBB621-14A8-4166-A87A-09C146F985A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27630" yWindow="330" windowWidth="25815" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vending_request_upload_template" sheetId="1" r:id="rId1"/>
@@ -381,7 +381,7 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,9 +438,12 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1000" xr:uid="{D4D81179-9F06-4B26-9BD4-C9995039BEA3}">
       <formula1>"profit, margin"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1000" xr:uid="{0DC2885B-6C8C-418A-A110-9219A6C72F59}">
+      <formula1>"Kayla Jones, John Narum, Ronnie Turner"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added loading message to upload
</commit_message>
<xml_diff>
--- a/public/vending-request-excel-template.xlsx
+++ b/public/vending-request-excel-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14234\OneDrive\Desktop\Web Dev\Projects\cti_blog\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BBB621-14A8-4166-A87A-09C146F985A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867E9F4F-FA21-4588-AC1D-580FBFEB6B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -381,7 +381,7 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>